<commit_message>
Add health cost tab
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/resume-nsf-pilot-01/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593DDA1B-B030-CA48-8B71-7FF2E282A466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B4AF61-E884-7D40-89A5-BA9B44975ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19400" yWindow="-21100" windowWidth="34560" windowHeight="19360" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="5000" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="parameters" sheetId="4" r:id="rId2"/>
-    <sheet name="jurisdiction" sheetId="2" r:id="rId3"/>
-    <sheet name="beta" sheetId="6" r:id="rId4"/>
-    <sheet name="travel" sheetId="3" r:id="rId5"/>
-    <sheet name="relative-mixing" sheetId="5" r:id="rId6"/>
+    <sheet name="health-costs" sheetId="7" r:id="rId3"/>
+    <sheet name="jurisdiction" sheetId="2" r:id="rId4"/>
+    <sheet name="beta" sheetId="6" r:id="rId5"/>
+    <sheet name="travel" sheetId="3" r:id="rId6"/>
+    <sheet name="relative-mixing" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="c_">parameters!$B$6</definedName>
@@ -130,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>setting</t>
   </si>
@@ -322,6 +323,33 @@
   </si>
   <si>
     <t>Percent reduction in IFR at the end of the pandemic.</t>
+  </si>
+  <si>
+    <t>chronic</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>severe</t>
+  </si>
+  <si>
+    <t>mild</t>
+  </si>
+  <si>
+    <t>hospital_cost</t>
+  </si>
+  <si>
+    <t>VSLY</t>
+  </si>
+  <si>
+    <t>disease_state_prevalence</t>
+  </si>
+  <si>
+    <t>disease_duration</t>
+  </si>
+  <si>
+    <t>DALY_weight</t>
   </si>
 </sst>
 </file>
@@ -795,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+    <sheetView zoomScale="141" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1076,6 +1104,126 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4AC197-751B-D642-B32A-DB1D08A8DC07}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.54</v>
+      </c>
+      <c r="E2">
+        <v>279113</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="C3">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.09</v>
+      </c>
+      <c r="E3">
+        <v>279113</v>
+      </c>
+      <c r="F3">
+        <v>11267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C4">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.03</v>
+      </c>
+      <c r="E4">
+        <v>279113</v>
+      </c>
+      <c r="F4">
+        <v>41510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>0.219</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.05</v>
+      </c>
+      <c r="E5">
+        <v>279113</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -1274,7 +1422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D10A5E8-0BB5-4C43-827E-A5AF4D063B7C}">
   <dimension ref="A1:T54"/>
   <sheetViews>
@@ -4798,7 +4946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40C96AD-7FCE-D24F-B326-0D5D7D33F358}">
   <dimension ref="A1:P43"/>
   <sheetViews>
@@ -6451,7 +6599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578CC606-5086-1F48-9D1A-C2900FAE3B19}">
   <dimension ref="A1:G7"/>
   <sheetViews>

</xml_diff>

<commit_message>
As per #9 read in the health cost params and calculate total cost per infection
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B4AF61-E884-7D40-89A5-BA9B44975ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B008025-2970-3F49-8921-7F8E0F2FDCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="620" yWindow="760" windowWidth="24940" windowHeight="17480" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="parameters" sheetId="4" r:id="rId2"/>
-    <sheet name="health-costs" sheetId="7" r:id="rId3"/>
+    <sheet name="healthcosts" sheetId="7" r:id="rId3"/>
     <sheet name="jurisdiction" sheetId="2" r:id="rId4"/>
     <sheet name="beta" sheetId="6" r:id="rId5"/>
     <sheet name="travel" sheetId="3" r:id="rId6"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>setting</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>DALY_weight</t>
+  </si>
+  <si>
+    <t>severity</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1111,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,9 +1122,14 @@
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="11" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
@@ -1203,6 +1211,7 @@
         <v>64</v>
       </c>
       <c r="B5">
+        <f>0.219</f>
         <v>0.219</v>
       </c>
       <c r="C5">

</xml_diff>

<commit_message>
Move VSLY to the parameters tab
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B008025-2970-3F49-8921-7F8E0F2FDCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28A9D16-60A8-2E4C-8B4D-BABE8FE309B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="760" windowWidth="24940" windowHeight="17480" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="840" yWindow="880" windowWidth="24940" windowHeight="15640" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="relative-mixing" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameters!$A$1:$G$24</definedName>
     <definedName name="c_">parameters!$B$6</definedName>
     <definedName name="C_surv">parameters!$B$12</definedName>
     <definedName name="days_to_adjust_NPI">parameters!$B$8</definedName>
@@ -32,6 +33,7 @@
     <definedName name="r_">parameters!$B$9</definedName>
     <definedName name="sigma">parameters!$B$2</definedName>
     <definedName name="tau">parameters!$B$5</definedName>
+    <definedName name="VSLY">parameters!$B$24</definedName>
     <definedName name="w">parameters!$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -131,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>setting</t>
   </si>
@@ -232,12 +234,6 @@
     <t>Cost of surveillance</t>
   </si>
   <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -353,6 +349,9 @@
   </si>
   <si>
     <t>severity</t>
+  </si>
+  <si>
+    <t>Value of a statistical life year</t>
   </si>
 </sst>
 </file>
@@ -784,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="181" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,14 +808,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -824,10 +815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A15" zoomScale="141" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,7 +861,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -907,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -934,10 +925,10 @@
         <v>0.01</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -976,131 +967,143 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>2.5</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7">
         <v>0.05</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="9">
         <v>0.02</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18">
         <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="11">
         <v>0.5</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="12">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="10">
         <f>0.7*2.38/1000/B15</f>
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="10">
         <f>B21*0.9</f>
         <v>7.4969999999999995E-2</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>1.5</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>279113</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G24" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -1108,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4AC197-751B-D642-B32A-DB1D08A8DC07}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,35 +1123,31 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" customWidth="1"/>
-    <col min="10" max="11" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
+    <col min="9" max="10" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>6.0000000000000001E-3</v>
@@ -1160,15 +1159,12 @@
         <v>0.54</v>
       </c>
       <c r="E2">
-        <v>279113</v>
-      </c>
-      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>0.13300000000000001</v>
@@ -1180,15 +1176,12 @@
         <v>0.09</v>
       </c>
       <c r="E3">
-        <v>279113</v>
-      </c>
-      <c r="F3">
         <v>11267</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>0.65500000000000003</v>
@@ -1200,15 +1193,12 @@
         <v>0.03</v>
       </c>
       <c r="E4">
-        <v>279113</v>
-      </c>
-      <c r="F4">
         <v>41510</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <f>0.219</f>
@@ -1221,9 +1211,6 @@
         <v>0.05</v>
       </c>
       <c r="E5">
-        <v>279113</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
     </row>
@@ -1265,7 +1252,7 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1318,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
As per #2 adding a coordination matrix
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28A9D16-60A8-2E4C-8B4D-BABE8FE309B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7189F8-46FD-1C4E-9E0C-A580E82C3AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="880" windowWidth="24940" windowHeight="15640" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="860" yWindow="1760" windowWidth="22080" windowHeight="15780" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="healthcosts" sheetId="7" r:id="rId3"/>
     <sheet name="jurisdiction" sheetId="2" r:id="rId4"/>
     <sheet name="beta" sheetId="6" r:id="rId5"/>
-    <sheet name="travel" sheetId="3" r:id="rId6"/>
-    <sheet name="relative-mixing" sheetId="5" r:id="rId7"/>
+    <sheet name="coordination" sheetId="8" r:id="rId6"/>
+    <sheet name="travel" sheetId="3" r:id="rId7"/>
+    <sheet name="relative-mixing" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameters!$A$1:$G$24</definedName>
@@ -110,6 +111,24 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D4FB1254-EC3E-B749-8D86-AF1DC61A85B4}</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{D4FB1254-EC3E-B749-8D86-AF1DC61A85B4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Do NOT EDIT UPPER RIGHT HAND (right of diagonal); They will AUTOMATICALLY mirror lower left</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -133,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>setting</t>
   </si>
@@ -352,6 +371,18 @@
   </si>
   <si>
     <t>Value of a statistical life year</t>
+  </si>
+  <si>
+    <t>YearsLostAtDeath</t>
+  </si>
+  <si>
+    <t>Number of Expected Life Years Lost to death from COVID</t>
+  </si>
+  <si>
+    <t>The probability that the disease event occurs (if it doesn't occur we just incur the surveillance cost).</t>
+  </si>
+  <si>
+    <t>p_disease_event</t>
   </si>
 </sst>
 </file>
@@ -451,6 +482,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Pedro Nascimento de Lima" id="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" userId="S::plima@rand.org::bad65025-c9fe-4811-b567-480395969e50" providerId="AD"/>
+  <person displayName="Sarah Karr" id="{FF1AC119-595F-EB42-B830-3D3539BE542F}" userId="S::sarahk@rand.org::6384f247-d4ff-499a-b2f3-dc408776128d" providerId="AD"/>
 </personList>
 </file>
 
@@ -781,12 +813,20 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E2" dT="2023-08-24T20:47:56.82" personId="{FF1AC119-595F-EB42-B830-3D3539BE542F}" id="{D4FB1254-EC3E-B749-8D86-AF1DC61A85B4}">
+    <text>Do NOT EDIT UPPER RIGHT HAND (right of diagonal); They will AUTOMATICALLY mirror lower left</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="181" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,10 +855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="141" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="141" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,7 +935,7 @@
         <v>22</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
@@ -906,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -914,7 +954,7 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1012,7 +1052,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1023,7 +1063,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1034,7 +1074,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1045,7 +1085,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1056,7 +1096,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1080,7 +1120,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1091,7 +1131,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1100,6 +1140,34 @@
       </c>
       <c r="C24" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25">
+        <v>13.8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1114,18 +1182,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="10" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1223,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="187" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="187" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4943,6 +5009,611 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2CF3C4-9881-3046-921C-4AF233771A62}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:T1">TRANSPOSE(A2:A20)</f>
+        <v>NY</v>
+      </c>
+      <c r="C1" t="str">
+        <v>NJ</v>
+      </c>
+      <c r="D1" t="str">
+        <v>PA</v>
+      </c>
+      <c r="E1" t="str">
+        <v/>
+      </c>
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
+      <c r="H1" t="str">
+        <v/>
+      </c>
+      <c r="I1" t="str">
+        <v/>
+      </c>
+      <c r="J1" t="str">
+        <v/>
+      </c>
+      <c r="K1" t="str">
+        <v/>
+      </c>
+      <c r="L1" t="str">
+        <v/>
+      </c>
+      <c r="M1" t="str">
+        <v/>
+      </c>
+      <c r="N1" t="str">
+        <v/>
+      </c>
+      <c r="O1" t="str">
+        <v/>
+      </c>
+      <c r="P1" t="str">
+        <v/>
+      </c>
+      <c r="Q1" t="str">
+        <v/>
+      </c>
+      <c r="R1" t="str">
+        <v/>
+      </c>
+      <c r="S1" t="str">
+        <v/>
+      </c>
+      <c r="T1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>IF(jurisdiction!B2="","",jurisdiction!B2)</f>
+        <v>NY</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(C2),ROW(C2)))="", "",INDIRECT(ADDRESS(COLUMN(C2),ROW(C2))))</f>
+        <v>0</v>
+      </c>
+      <c r="D2" cm="1">
+        <f t="array" aca="1" ref="D2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(D2),ROW(D2)))="", "",INDIRECT(ADDRESS(COLUMN(D2),ROW(D2))))</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str" cm="1">
+        <f t="array" aca="1" ref="E2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(E2),ROW(E2)))="", "",INDIRECT(ADDRESS(COLUMN(E2),ROW(E2))))</f>
+        <v/>
+      </c>
+      <c r="F2" t="str" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(F2),ROW(F2)))="", "",INDIRECT(ADDRESS(COLUMN(F2),ROW(F2))))</f>
+        <v/>
+      </c>
+      <c r="G2" t="str" cm="1">
+        <f t="array" aca="1" ref="G2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(G2),ROW(G2)))="", "",INDIRECT(ADDRESS(COLUMN(G2),ROW(G2))))</f>
+        <v/>
+      </c>
+      <c r="H2" t="str" cm="1">
+        <f t="array" aca="1" ref="H2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(H2),ROW(H2)))="", "",INDIRECT(ADDRESS(COLUMN(H2),ROW(H2))))</f>
+        <v/>
+      </c>
+      <c r="I2" t="str" cm="1">
+        <f t="array" aca="1" ref="I2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I2),ROW(I2)))="", "",INDIRECT(ADDRESS(COLUMN(I2),ROW(I2))))</f>
+        <v/>
+      </c>
+      <c r="J2" t="str" cm="1">
+        <f t="array" aca="1" ref="J2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J2),ROW(J2)))="", "",INDIRECT(ADDRESS(COLUMN(J2),ROW(J2))))</f>
+        <v/>
+      </c>
+      <c r="K2" t="str" cm="1">
+        <f t="array" aca="1" ref="K2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K2),ROW(K2)))="", "",INDIRECT(ADDRESS(COLUMN(K2),ROW(K2))))</f>
+        <v/>
+      </c>
+      <c r="L2" t="str" cm="1">
+        <f t="array" aca="1" ref="L2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L2),ROW(L2)))="", "",INDIRECT(ADDRESS(COLUMN(L2),ROW(L2))))</f>
+        <v/>
+      </c>
+      <c r="M2" t="str" cm="1">
+        <f t="array" aca="1" ref="M2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M2),ROW(M2)))="", "",INDIRECT(ADDRESS(COLUMN(M2),ROW(M2))))</f>
+        <v/>
+      </c>
+      <c r="N2" t="str" cm="1">
+        <f t="array" aca="1" ref="N2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N2),ROW(N2)))="", "",INDIRECT(ADDRESS(COLUMN(N2),ROW(N2))))</f>
+        <v/>
+      </c>
+      <c r="O2" t="str" cm="1">
+        <f t="array" aca="1" ref="O2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O2),ROW(O2)))="", "",INDIRECT(ADDRESS(COLUMN(O2),ROW(O2))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>IF(jurisdiction!B3="","",jurisdiction!B3)</f>
+        <v>NJ</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(D3),ROW(D3)))="", "",INDIRECT(ADDRESS(COLUMN(D3),ROW(D3))))</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="str" cm="1">
+        <f t="array" aca="1" ref="E3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(E3),ROW(E3)))="", "",INDIRECT(ADDRESS(COLUMN(E3),ROW(E3))))</f>
+        <v/>
+      </c>
+      <c r="F3" t="str" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(F3),ROW(F3)))="", "",INDIRECT(ADDRESS(COLUMN(F3),ROW(F3))))</f>
+        <v/>
+      </c>
+      <c r="G3" t="str" cm="1">
+        <f t="array" aca="1" ref="G3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(G3),ROW(G3)))="", "",INDIRECT(ADDRESS(COLUMN(G3),ROW(G3))))</f>
+        <v/>
+      </c>
+      <c r="H3" t="str" cm="1">
+        <f t="array" aca="1" ref="H3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(H3),ROW(H3)))="", "",INDIRECT(ADDRESS(COLUMN(H3),ROW(H3))))</f>
+        <v/>
+      </c>
+      <c r="I3" t="str" cm="1">
+        <f t="array" aca="1" ref="I3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I3),ROW(I3)))="", "",INDIRECT(ADDRESS(COLUMN(I3),ROW(I3))))</f>
+        <v/>
+      </c>
+      <c r="J3" t="str" cm="1">
+        <f t="array" aca="1" ref="J3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J3),ROW(J3)))="", "",INDIRECT(ADDRESS(COLUMN(J3),ROW(J3))))</f>
+        <v/>
+      </c>
+      <c r="K3" t="str" cm="1">
+        <f t="array" aca="1" ref="K3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K3),ROW(K3)))="", "",INDIRECT(ADDRESS(COLUMN(K3),ROW(K3))))</f>
+        <v/>
+      </c>
+      <c r="L3" t="str" cm="1">
+        <f t="array" aca="1" ref="L3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L3),ROW(L3)))="", "",INDIRECT(ADDRESS(COLUMN(L3),ROW(L3))))</f>
+        <v/>
+      </c>
+      <c r="M3" t="str" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M3),ROW(M3)))="", "",INDIRECT(ADDRESS(COLUMN(M3),ROW(M3))))</f>
+        <v/>
+      </c>
+      <c r="N3" t="str" cm="1">
+        <f t="array" aca="1" ref="N3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N3),ROW(N3)))="", "",INDIRECT(ADDRESS(COLUMN(N3),ROW(N3))))</f>
+        <v/>
+      </c>
+      <c r="O3" t="str" cm="1">
+        <f t="array" aca="1" ref="O3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O3),ROW(O3)))="", "",INDIRECT(ADDRESS(COLUMN(O3),ROW(O3))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>IF(jurisdiction!B4="","",jurisdiction!B4)</f>
+        <v>PA</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str" cm="1">
+        <f t="array" aca="1" ref="E4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(E4),ROW(E4)))="", "",INDIRECT(ADDRESS(COLUMN(E4),ROW(E4))))</f>
+        <v/>
+      </c>
+      <c r="F4" t="str" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(F4),ROW(F4)))="", "",INDIRECT(ADDRESS(COLUMN(F4),ROW(F4))))</f>
+        <v/>
+      </c>
+      <c r="G4" t="str" cm="1">
+        <f t="array" aca="1" ref="G4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(G4),ROW(G4)))="", "",INDIRECT(ADDRESS(COLUMN(G4),ROW(G4))))</f>
+        <v/>
+      </c>
+      <c r="H4" t="str" cm="1">
+        <f t="array" aca="1" ref="H4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(H4),ROW(H4)))="", "",INDIRECT(ADDRESS(COLUMN(H4),ROW(H4))))</f>
+        <v/>
+      </c>
+      <c r="I4" t="str" cm="1">
+        <f t="array" aca="1" ref="I4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I4),ROW(I4)))="", "",INDIRECT(ADDRESS(COLUMN(I4),ROW(I4))))</f>
+        <v/>
+      </c>
+      <c r="J4" t="str" cm="1">
+        <f t="array" aca="1" ref="J4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J4),ROW(J4)))="", "",INDIRECT(ADDRESS(COLUMN(J4),ROW(J4))))</f>
+        <v/>
+      </c>
+      <c r="K4" t="str" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K4),ROW(K4)))="", "",INDIRECT(ADDRESS(COLUMN(K4),ROW(K4))))</f>
+        <v/>
+      </c>
+      <c r="L4" t="str" cm="1">
+        <f t="array" aca="1" ref="L4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L4),ROW(L4)))="", "",INDIRECT(ADDRESS(COLUMN(L4),ROW(L4))))</f>
+        <v/>
+      </c>
+      <c r="M4" t="str" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M4),ROW(M4)))="", "",INDIRECT(ADDRESS(COLUMN(M4),ROW(M4))))</f>
+        <v/>
+      </c>
+      <c r="N4" t="str" cm="1">
+        <f t="array" aca="1" ref="N4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N4),ROW(N4)))="", "",INDIRECT(ADDRESS(COLUMN(N4),ROW(N4))))</f>
+        <v/>
+      </c>
+      <c r="O4" t="str" cm="1">
+        <f t="array" aca="1" ref="O4" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O4),ROW(O4)))="", "",INDIRECT(ADDRESS(COLUMN(O4),ROW(O4))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>IF(jurisdiction!B5="","",jurisdiction!B5)</f>
+        <v/>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(F5),ROW(F5)))="", "",INDIRECT(ADDRESS(COLUMN(F5),ROW(F5))))</f>
+        <v/>
+      </c>
+      <c r="G5" t="str" cm="1">
+        <f t="array" aca="1" ref="G5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(G5),ROW(G5)))="", "",INDIRECT(ADDRESS(COLUMN(G5),ROW(G5))))</f>
+        <v/>
+      </c>
+      <c r="H5" t="str" cm="1">
+        <f t="array" aca="1" ref="H5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(H5),ROW(H5)))="", "",INDIRECT(ADDRESS(COLUMN(H5),ROW(H5))))</f>
+        <v/>
+      </c>
+      <c r="I5" t="str" cm="1">
+        <f t="array" aca="1" ref="I5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I5),ROW(I5)))="", "",INDIRECT(ADDRESS(COLUMN(I5),ROW(I5))))</f>
+        <v/>
+      </c>
+      <c r="J5" t="str" cm="1">
+        <f t="array" aca="1" ref="J5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J5),ROW(J5)))="", "",INDIRECT(ADDRESS(COLUMN(J5),ROW(J5))))</f>
+        <v/>
+      </c>
+      <c r="K5" t="str" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K5),ROW(K5)))="", "",INDIRECT(ADDRESS(COLUMN(K5),ROW(K5))))</f>
+        <v/>
+      </c>
+      <c r="L5" t="str" cm="1">
+        <f t="array" aca="1" ref="L5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L5),ROW(L5)))="", "",INDIRECT(ADDRESS(COLUMN(L5),ROW(L5))))</f>
+        <v/>
+      </c>
+      <c r="M5" t="str" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M5),ROW(M5)))="", "",INDIRECT(ADDRESS(COLUMN(M5),ROW(M5))))</f>
+        <v/>
+      </c>
+      <c r="N5" t="str" cm="1">
+        <f t="array" aca="1" ref="N5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N5),ROW(N5)))="", "",INDIRECT(ADDRESS(COLUMN(N5),ROW(N5))))</f>
+        <v/>
+      </c>
+      <c r="O5" t="str" cm="1">
+        <f t="array" aca="1" ref="O5" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O5),ROW(O5)))="", "",INDIRECT(ADDRESS(COLUMN(O5),ROW(O5))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>IF(jurisdiction!B6="","",jurisdiction!B6)</f>
+        <v/>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(G6),ROW(G6)))="", "",INDIRECT(ADDRESS(COLUMN(G6),ROW(G6))))</f>
+        <v/>
+      </c>
+      <c r="H6" t="str" cm="1">
+        <f t="array" aca="1" ref="H6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(H6),ROW(H6)))="", "",INDIRECT(ADDRESS(COLUMN(H6),ROW(H6))))</f>
+        <v/>
+      </c>
+      <c r="I6" t="str" cm="1">
+        <f t="array" aca="1" ref="I6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I6),ROW(I6)))="", "",INDIRECT(ADDRESS(COLUMN(I6),ROW(I6))))</f>
+        <v/>
+      </c>
+      <c r="J6" t="str" cm="1">
+        <f t="array" aca="1" ref="J6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J6),ROW(J6)))="", "",INDIRECT(ADDRESS(COLUMN(J6),ROW(J6))))</f>
+        <v/>
+      </c>
+      <c r="K6" t="str" cm="1">
+        <f t="array" aca="1" ref="K6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K6),ROW(K6)))="", "",INDIRECT(ADDRESS(COLUMN(K6),ROW(K6))))</f>
+        <v/>
+      </c>
+      <c r="L6" t="str" cm="1">
+        <f t="array" aca="1" ref="L6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L6),ROW(L6)))="", "",INDIRECT(ADDRESS(COLUMN(L6),ROW(L6))))</f>
+        <v/>
+      </c>
+      <c r="M6" t="str" cm="1">
+        <f t="array" aca="1" ref="M6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M6),ROW(M6)))="", "",INDIRECT(ADDRESS(COLUMN(M6),ROW(M6))))</f>
+        <v/>
+      </c>
+      <c r="N6" t="str" cm="1">
+        <f t="array" aca="1" ref="N6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N6),ROW(N6)))="", "",INDIRECT(ADDRESS(COLUMN(N6),ROW(N6))))</f>
+        <v/>
+      </c>
+      <c r="O6" t="str" cm="1">
+        <f t="array" aca="1" ref="O6" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O6),ROW(O6)))="", "",INDIRECT(ADDRESS(COLUMN(O6),ROW(O6))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>IF(jurisdiction!B7="","",jurisdiction!B7)</f>
+        <v/>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="str" cm="1">
+        <f t="array" aca="1" ref="H7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(H7),ROW(H7)))="", "",INDIRECT(ADDRESS(COLUMN(H7),ROW(H7))))</f>
+        <v/>
+      </c>
+      <c r="I7" t="str" cm="1">
+        <f t="array" aca="1" ref="I7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I7),ROW(I7)))="", "",INDIRECT(ADDRESS(COLUMN(I7),ROW(I7))))</f>
+        <v/>
+      </c>
+      <c r="J7" t="str" cm="1">
+        <f t="array" aca="1" ref="J7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J7),ROW(J7)))="", "",INDIRECT(ADDRESS(COLUMN(J7),ROW(J7))))</f>
+        <v/>
+      </c>
+      <c r="K7" t="str" cm="1">
+        <f t="array" aca="1" ref="K7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K7),ROW(K7)))="", "",INDIRECT(ADDRESS(COLUMN(K7),ROW(K7))))</f>
+        <v/>
+      </c>
+      <c r="L7" t="str" cm="1">
+        <f t="array" aca="1" ref="L7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L7),ROW(L7)))="", "",INDIRECT(ADDRESS(COLUMN(L7),ROW(L7))))</f>
+        <v/>
+      </c>
+      <c r="M7" t="str" cm="1">
+        <f t="array" aca="1" ref="M7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M7),ROW(M7)))="", "",INDIRECT(ADDRESS(COLUMN(M7),ROW(M7))))</f>
+        <v/>
+      </c>
+      <c r="N7" t="str" cm="1">
+        <f t="array" aca="1" ref="N7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N7),ROW(N7)))="", "",INDIRECT(ADDRESS(COLUMN(N7),ROW(N7))))</f>
+        <v/>
+      </c>
+      <c r="O7" t="str" cm="1">
+        <f t="array" aca="1" ref="O7" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O7),ROW(O7)))="", "",INDIRECT(ADDRESS(COLUMN(O7),ROW(O7))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>IF(jurisdiction!B8="","",jurisdiction!B8)</f>
+        <v/>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="str" cm="1">
+        <f t="array" aca="1" ref="I8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(I8),ROW(I8)))="", "",INDIRECT(ADDRESS(COLUMN(I8),ROW(I8))))</f>
+        <v/>
+      </c>
+      <c r="J8" t="str" cm="1">
+        <f t="array" aca="1" ref="J8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J8),ROW(J8)))="", "",INDIRECT(ADDRESS(COLUMN(J8),ROW(J8))))</f>
+        <v/>
+      </c>
+      <c r="K8" t="str" cm="1">
+        <f t="array" aca="1" ref="K8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K8),ROW(K8)))="", "",INDIRECT(ADDRESS(COLUMN(K8),ROW(K8))))</f>
+        <v/>
+      </c>
+      <c r="L8" t="str" cm="1">
+        <f t="array" aca="1" ref="L8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L8),ROW(L8)))="", "",INDIRECT(ADDRESS(COLUMN(L8),ROW(L8))))</f>
+        <v/>
+      </c>
+      <c r="M8" t="str" cm="1">
+        <f t="array" aca="1" ref="M8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M8),ROW(M8)))="", "",INDIRECT(ADDRESS(COLUMN(M8),ROW(M8))))</f>
+        <v/>
+      </c>
+      <c r="N8" t="str" cm="1">
+        <f t="array" aca="1" ref="N8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N8),ROW(N8)))="", "",INDIRECT(ADDRESS(COLUMN(N8),ROW(N8))))</f>
+        <v/>
+      </c>
+      <c r="O8" t="str" cm="1">
+        <f t="array" aca="1" ref="O8" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O8),ROW(O8)))="", "",INDIRECT(ADDRESS(COLUMN(O8),ROW(O8))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>IF(jurisdiction!B9="","",jurisdiction!B9)</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="str" cm="1">
+        <f t="array" aca="1" ref="J9" ca="1">IF(INDIRECT(ADDRESS(COLUMN(J9),ROW(J9)))="", "",INDIRECT(ADDRESS(COLUMN(J9),ROW(J9))))</f>
+        <v/>
+      </c>
+      <c r="K9" t="str" cm="1">
+        <f t="array" aca="1" ref="K9" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K9),ROW(K9)))="", "",INDIRECT(ADDRESS(COLUMN(K9),ROW(K9))))</f>
+        <v/>
+      </c>
+      <c r="L9" t="str" cm="1">
+        <f t="array" aca="1" ref="L9" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L9),ROW(L9)))="", "",INDIRECT(ADDRESS(COLUMN(L9),ROW(L9))))</f>
+        <v/>
+      </c>
+      <c r="M9" t="str" cm="1">
+        <f t="array" aca="1" ref="M9" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M9),ROW(M9)))="", "",INDIRECT(ADDRESS(COLUMN(M9),ROW(M9))))</f>
+        <v/>
+      </c>
+      <c r="N9" t="str" cm="1">
+        <f t="array" aca="1" ref="N9" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N9),ROW(N9)))="", "",INDIRECT(ADDRESS(COLUMN(N9),ROW(N9))))</f>
+        <v/>
+      </c>
+      <c r="O9" t="str" cm="1">
+        <f t="array" aca="1" ref="O9" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O9),ROW(O9)))="", "",INDIRECT(ADDRESS(COLUMN(O9),ROW(O9))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>IF(jurisdiction!B10="","",jurisdiction!B10)</f>
+        <v/>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="str" cm="1">
+        <f t="array" aca="1" ref="K10" ca="1">IF(INDIRECT(ADDRESS(COLUMN(K10),ROW(K10)))="", "",INDIRECT(ADDRESS(COLUMN(K10),ROW(K10))))</f>
+        <v/>
+      </c>
+      <c r="L10" t="str" cm="1">
+        <f t="array" aca="1" ref="L10" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L10),ROW(L10)))="", "",INDIRECT(ADDRESS(COLUMN(L10),ROW(L10))))</f>
+        <v/>
+      </c>
+      <c r="M10" t="str" cm="1">
+        <f t="array" aca="1" ref="M10" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M10),ROW(M10)))="", "",INDIRECT(ADDRESS(COLUMN(M10),ROW(M10))))</f>
+        <v/>
+      </c>
+      <c r="N10" t="str" cm="1">
+        <f t="array" aca="1" ref="N10" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N10),ROW(N10)))="", "",INDIRECT(ADDRESS(COLUMN(N10),ROW(N10))))</f>
+        <v/>
+      </c>
+      <c r="O10" t="str" cm="1">
+        <f t="array" aca="1" ref="O10" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O10),ROW(O10)))="", "",INDIRECT(ADDRESS(COLUMN(O10),ROW(O10))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>IF(jurisdiction!B11="","",jurisdiction!B11)</f>
+        <v/>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="str" cm="1">
+        <f t="array" aca="1" ref="L11" ca="1">IF(INDIRECT(ADDRESS(COLUMN(L11),ROW(L11)))="", "",INDIRECT(ADDRESS(COLUMN(L11),ROW(L11))))</f>
+        <v/>
+      </c>
+      <c r="M11" t="str" cm="1">
+        <f t="array" aca="1" ref="M11" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M11),ROW(M11)))="", "",INDIRECT(ADDRESS(COLUMN(M11),ROW(M11))))</f>
+        <v/>
+      </c>
+      <c r="N11" t="str" cm="1">
+        <f t="array" aca="1" ref="N11" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N11),ROW(N11)))="", "",INDIRECT(ADDRESS(COLUMN(N11),ROW(N11))))</f>
+        <v/>
+      </c>
+      <c r="O11" t="str" cm="1">
+        <f t="array" aca="1" ref="O11" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O11),ROW(O11)))="", "",INDIRECT(ADDRESS(COLUMN(O11),ROW(O11))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>IF(jurisdiction!B12="","",jurisdiction!B12)</f>
+        <v/>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" t="str" cm="1">
+        <f t="array" aca="1" ref="M12" ca="1">IF(INDIRECT(ADDRESS(COLUMN(M12),ROW(M12)))="", "",INDIRECT(ADDRESS(COLUMN(M12),ROW(M12))))</f>
+        <v/>
+      </c>
+      <c r="N12" t="str" cm="1">
+        <f t="array" aca="1" ref="N12" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N12),ROW(N12)))="", "",INDIRECT(ADDRESS(COLUMN(N12),ROW(N12))))</f>
+        <v/>
+      </c>
+      <c r="O12" t="str" cm="1">
+        <f t="array" aca="1" ref="O12" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O12),ROW(O12)))="", "",INDIRECT(ADDRESS(COLUMN(O12),ROW(O12))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>IF(jurisdiction!B13="","",jurisdiction!B13)</f>
+        <v/>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="str" cm="1">
+        <f t="array" aca="1" ref="N13" ca="1">IF(INDIRECT(ADDRESS(COLUMN(N13),ROW(N13)))="", "",INDIRECT(ADDRESS(COLUMN(N13),ROW(N13))))</f>
+        <v/>
+      </c>
+      <c r="O13" t="str" cm="1">
+        <f t="array" aca="1" ref="O13" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O13),ROW(O13)))="", "",INDIRECT(ADDRESS(COLUMN(O13),ROW(O13))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>IF(jurisdiction!B14="","",jurisdiction!B14)</f>
+        <v/>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="str" cm="1">
+        <f t="array" aca="1" ref="O14" ca="1">IF(INDIRECT(ADDRESS(COLUMN(O14),ROW(O14)))="", "",INDIRECT(ADDRESS(COLUMN(O14),ROW(O14))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>IF(jurisdiction!B15="","",jurisdiction!B15)</f>
+        <v/>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>IF(jurisdiction!B16="","",jurisdiction!B16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f>IF(jurisdiction!B17="","",jurisdiction!B17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f>IF(jurisdiction!B18="","",jurisdiction!B18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f>IF(jurisdiction!B19="","",jurisdiction!B19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f>IF(jurisdiction!B20="","",jurisdiction!B20)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40C96AD-7FCE-D24F-B326-0D5D7D33F358}">
   <dimension ref="A1:P43"/>
   <sheetViews>
@@ -6595,22 +7266,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578CC606-5086-1F48-9D1A-C2900FAE3B19}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="A5" sqref="A5:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:G1">TRANSPOSE(A2:A7)</f>
+        <f t="array" ref="B1:T1">TRANSPOSE(A2:A20)</f>
         <v>NY</v>
       </c>
       <c r="C1" t="str">
@@ -6619,19 +7290,58 @@
       <c r="D1" t="str">
         <v>PA</v>
       </c>
-      <c r="E1">
+      <c r="E1" t="str">
+        <v/>
+      </c>
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
+      <c r="H1" t="str">
+        <v/>
+      </c>
+      <c r="I1" t="str">
+        <v/>
+      </c>
+      <c r="J1" t="str">
+        <v/>
+      </c>
+      <c r="K1" t="str">
+        <v/>
+      </c>
+      <c r="L1" t="str">
+        <v/>
+      </c>
+      <c r="M1" t="str">
+        <v/>
+      </c>
+      <c r="N1" t="str">
+        <v/>
+      </c>
+      <c r="O1" t="str">
+        <v/>
+      </c>
+      <c r="P1" t="str">
+        <v/>
+      </c>
+      <c r="Q1">
         <v>0</v>
       </c>
-      <c r="F1">
+      <c r="R1">
         <v>0</v>
       </c>
-      <c r="G1">
+      <c r="S1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="T1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>jurisdiction!B2</f>
+        <f>IF(jurisdiction!B2="","",jurisdiction!B2)</f>
         <v>NY</v>
       </c>
       <c r="B2" s="1">
@@ -6653,9 +7363,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>jurisdiction!B3</f>
+        <f>IF(jurisdiction!B3="","",jurisdiction!B3)</f>
         <v>NJ</v>
       </c>
       <c r="B3" s="1">
@@ -6677,9 +7387,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>jurisdiction!B4</f>
+        <f>IF(jurisdiction!B4="","",jurisdiction!B4)</f>
         <v>PA</v>
       </c>
       <c r="B4" s="1">
@@ -6701,10 +7411,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f>jurisdiction!B5</f>
-        <v>0</v>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>IF(jurisdiction!B5="","",jurisdiction!B5)</f>
+        <v/>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -6725,10 +7435,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f>jurisdiction!B6</f>
-        <v>0</v>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>IF(jurisdiction!B6="","",jurisdiction!B6)</f>
+        <v/>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -6749,10 +7459,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f>jurisdiction!B7</f>
-        <v>0</v>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>IF(jurisdiction!B7="","",jurisdiction!B7)</f>
+        <v/>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -6771,6 +7481,60 @@
       </c>
       <c r="G7" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>IF(jurisdiction!B8="","",jurisdiction!B8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>IF(jurisdiction!B9="","",jurisdiction!B9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>IF(jurisdiction!B10="","",jurisdiction!B10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>IF(jurisdiction!B11="","",jurisdiction!B11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>IF(jurisdiction!B12="","",jurisdiction!B12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>IF(jurisdiction!B13="","",jurisdiction!B13)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>IF(jurisdiction!B14="","",jurisdiction!B14)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>IF(jurisdiction!B15="","",jurisdiction!B15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>IF(jurisdiction!B16="","",jurisdiction!B16)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
npi coordination working implementation with max and avg option for #2
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7189F8-46FD-1C4E-9E0C-A580E82C3AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90B4CB-3E27-A545-958D-3BA7381DAC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1760" windowWidth="22080" windowHeight="15780" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="5" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="141" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView zoomScale="141" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="187" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,6 +1299,7 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1489,7 +1490,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5012,9 +5013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2CF3C4-9881-3046-921C-4AF233771A62}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -5086,12 +5085,10 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" cm="1">
-        <f t="array" aca="1" ref="C2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(C2),ROW(C2)))="", "",INDIRECT(ADDRESS(COLUMN(C2),ROW(C2))))</f>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" cm="1">
-        <f t="array" aca="1" ref="D2" ca="1">IF(INDIRECT(ADDRESS(COLUMN(D2),ROW(D2)))="", "",INDIRECT(ADDRESS(COLUMN(D2),ROW(D2))))</f>
+      <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="str" cm="1">
@@ -5150,9 +5147,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" cm="1">
-        <f t="array" aca="1" ref="D3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(D3),ROW(D3)))="", "",INDIRECT(ADDRESS(COLUMN(D3),ROW(D3))))</f>
-        <v>1</v>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3" t="str" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">IF(INDIRECT(ADDRESS(COLUMN(E3),ROW(E3)))="", "",INDIRECT(ADDRESS(COLUMN(E3),ROW(E3))))</f>
@@ -5208,7 +5204,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>

<commit_message>
wip changes to allow larger experiments
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90B4CB-3E27-A545-958D-3BA7381DAC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8D31F8-64A3-274D-9D9F-BAE93F3C0D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="5" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="3" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>setting</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>p_disease_event</t>
+  </si>
+  <si>
+    <t>Number of simulation patches</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1170,6 +1173,18 @@
         <v>75</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <f>MAX(jurisdiction!A:A)</f>
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G24" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1182,7 +1197,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1289,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5013,7 +5028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2CF3C4-9881-3046-921C-4AF233771A62}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
model now runs again, major modifications to how inputs are set
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8D31F8-64A3-274D-9D9F-BAE93F3C0D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2CC4FB-C343-D94B-B96D-1954599D8FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="3" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="4" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="parameters" sheetId="4" r:id="rId2"/>
     <sheet name="healthcosts" sheetId="7" r:id="rId3"/>
     <sheet name="jurisdiction" sheetId="2" r:id="rId4"/>
-    <sheet name="beta" sheetId="6" r:id="rId5"/>
+    <sheet name="beta_raw" sheetId="6" r:id="rId5"/>
     <sheet name="coordination" sheetId="8" r:id="rId6"/>
     <sheet name="travel" sheetId="3" r:id="rId7"/>
     <sheet name="relative-mixing" sheetId="5" r:id="rId8"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>setting</t>
   </si>
@@ -386,6 +386,24 @@
   </si>
   <si>
     <t>Number of simulation patches</t>
+  </si>
+  <si>
+    <t>npi_coord_max</t>
+  </si>
+  <si>
+    <t>1 if using max value of NPI strategies, 0 if using weighted sum</t>
+  </si>
+  <si>
+    <t>npi_duration</t>
+  </si>
+  <si>
+    <t>number of days through which NPIs will be used</t>
+  </si>
+  <si>
+    <t>trans_mult</t>
+  </si>
+  <si>
+    <t>transmissibility multiplicative factor used for scenario analysis. Multiplies over the beta matrix.</t>
   </si>
 </sst>
 </file>
@@ -858,10 +876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1183,6 +1201,39 @@
       </c>
       <c r="C27" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29">
+        <v>1000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+    <sheetView zoomScale="187" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1504,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D10A5E8-0BB5-4C43-827E-A5AF4D063B7C}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5636,73 +5687,73 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>IF(beta!A1="","",beta!A1)</f>
+        <f>IF(beta_raw!A1="","",beta_raw!A1)</f>
         <v>jurisdiction</v>
       </c>
       <c r="B1" t="str">
-        <f>beta!B1</f>
+        <f>beta_raw!B1</f>
         <v>NY</v>
       </c>
       <c r="C1" t="str">
-        <f>beta!C1</f>
+        <f>beta_raw!C1</f>
         <v>NJ</v>
       </c>
       <c r="D1" t="str">
-        <f>beta!D1</f>
+        <f>beta_raw!D1</f>
         <v>PA</v>
       </c>
       <c r="E1" t="str">
-        <f>beta!E1</f>
+        <f>beta_raw!E1</f>
         <v/>
       </c>
       <c r="F1" t="str">
-        <f>beta!F1</f>
+        <f>beta_raw!F1</f>
         <v/>
       </c>
       <c r="G1" t="str">
-        <f>beta!G1</f>
+        <f>beta_raw!G1</f>
         <v/>
       </c>
       <c r="H1" t="str">
-        <f>beta!H1</f>
+        <f>beta_raw!H1</f>
         <v/>
       </c>
       <c r="I1" t="str">
-        <f>beta!I1</f>
+        <f>beta_raw!I1</f>
         <v/>
       </c>
       <c r="J1" t="str">
-        <f>beta!J1</f>
+        <f>beta_raw!J1</f>
         <v/>
       </c>
       <c r="K1" t="str">
-        <f>beta!K1</f>
+        <f>beta_raw!K1</f>
         <v/>
       </c>
       <c r="L1" t="str">
-        <f>beta!L1</f>
+        <f>beta_raw!L1</f>
         <v/>
       </c>
       <c r="M1" t="str">
-        <f>beta!M1</f>
+        <f>beta_raw!M1</f>
         <v/>
       </c>
       <c r="N1" t="str">
-        <f>beta!N1</f>
+        <f>beta_raw!N1</f>
         <v/>
       </c>
       <c r="O1" t="str">
-        <f>beta!O1</f>
+        <f>beta_raw!O1</f>
         <v/>
       </c>
       <c r="P1" t="str">
-        <f>beta!P1</f>
+        <f>beta_raw!P1</f>
         <v/>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>IF(beta!A2="","",beta!A2)</f>
+        <f>IF(beta_raw!A2="","",beta_raw!A2)</f>
         <v>NY</v>
       </c>
       <c r="B2">
@@ -5752,7 +5803,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>IF(beta!A3="","",beta!A3)</f>
+        <f>IF(beta_raw!A3="","",beta_raw!A3)</f>
         <v>NJ</v>
       </c>
       <c r="B3">
@@ -5802,7 +5853,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>IF(beta!A4="","",beta!A4)</f>
+        <f>IF(beta_raw!A4="","",beta_raw!A4)</f>
         <v>PA</v>
       </c>
       <c r="B4">
@@ -5852,7 +5903,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>IF(beta!A5="","",beta!A5)</f>
+        <f>IF(beta_raw!A5="","",beta_raw!A5)</f>
         <v/>
       </c>
       <c r="B5" t="str">
@@ -5902,7 +5953,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>IF(beta!A6="","",beta!A6)</f>
+        <f>IF(beta_raw!A6="","",beta_raw!A6)</f>
         <v/>
       </c>
       <c r="B6" t="str">
@@ -5952,7 +6003,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>IF(beta!A7="","",beta!A7)</f>
+        <f>IF(beta_raw!A7="","",beta_raw!A7)</f>
         <v/>
       </c>
       <c r="B7" t="str">
@@ -6002,7 +6053,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>IF(beta!A8="","",beta!A8)</f>
+        <f>IF(beta_raw!A8="","",beta_raw!A8)</f>
         <v/>
       </c>
       <c r="B8" t="str">
@@ -6052,7 +6103,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>IF(beta!A9="","",beta!A9)</f>
+        <f>IF(beta_raw!A9="","",beta_raw!A9)</f>
         <v/>
       </c>
       <c r="B9" t="str">
@@ -6102,7 +6153,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>IF(beta!A10="","",beta!A10)</f>
+        <f>IF(beta_raw!A10="","",beta_raw!A10)</f>
         <v/>
       </c>
       <c r="B10" t="str">
@@ -6152,7 +6203,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>IF(beta!A11="","",beta!A11)</f>
+        <f>IF(beta_raw!A11="","",beta_raw!A11)</f>
         <v/>
       </c>
       <c r="B11" t="str">
@@ -6202,7 +6253,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>IF(beta!A12="","",beta!A12)</f>
+        <f>IF(beta_raw!A12="","",beta_raw!A12)</f>
         <v/>
       </c>
       <c r="B12" t="str">
@@ -6252,7 +6303,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>IF(beta!A13="","",beta!A13)</f>
+        <f>IF(beta_raw!A13="","",beta_raw!A13)</f>
         <v/>
       </c>
       <c r="B13" t="str">
@@ -6302,7 +6353,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>IF(beta!A14="","",beta!A14)</f>
+        <f>IF(beta_raw!A14="","",beta_raw!A14)</f>
         <v/>
       </c>
       <c r="B14" t="str">
@@ -6352,7 +6403,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>IF(beta!A15="","",beta!A15)</f>
+        <f>IF(beta_raw!A15="","",beta_raw!A15)</f>
         <v/>
       </c>
       <c r="B15" t="str">
@@ -6402,7 +6453,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>IF(beta!A16="","",beta!A16)</f>
+        <f>IF(beta_raw!A16="","",beta_raw!A16)</f>
         <v/>
       </c>
       <c r="B16" t="str">
@@ -6452,7 +6503,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>IF(beta!A17="","",beta!A17)</f>
+        <f>IF(beta_raw!A17="","",beta_raw!A17)</f>
         <v/>
       </c>
       <c r="B17" t="str">
@@ -6502,7 +6553,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>IF(beta!A18="","",beta!A18)</f>
+        <f>IF(beta_raw!A18="","",beta_raw!A18)</f>
         <v/>
       </c>
       <c r="B18" t="str">
@@ -6552,7 +6603,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>IF(beta!A19="","",beta!A19)</f>
+        <f>IF(beta_raw!A19="","",beta_raw!A19)</f>
         <v/>
       </c>
       <c r="B19" t="str">
@@ -6602,7 +6653,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>IF(beta!A20="","",beta!A20)</f>
+        <f>IF(beta_raw!A20="","",beta_raw!A20)</f>
         <v/>
       </c>
       <c r="B20" t="str">
@@ -6652,7 +6703,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>IF(beta!A21="","",beta!A21)</f>
+        <f>IF(beta_raw!A21="","",beta_raw!A21)</f>
         <v/>
       </c>
       <c r="B21" t="str">
@@ -6702,7 +6753,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>IF(beta!A22="","",beta!A22)</f>
+        <f>IF(beta_raw!A22="","",beta_raw!A22)</f>
         <v/>
       </c>
       <c r="B22" t="str">
@@ -6752,7 +6803,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>IF(beta!A23="","",beta!A23)</f>
+        <f>IF(beta_raw!A23="","",beta_raw!A23)</f>
         <v/>
       </c>
       <c r="B23" t="str">
@@ -6802,7 +6853,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>IF(beta!A24="","",beta!A24)</f>
+        <f>IF(beta_raw!A24="","",beta_raw!A24)</f>
         <v/>
       </c>
       <c r="B24" t="str">
@@ -6852,7 +6903,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>IF(beta!A25="","",beta!A25)</f>
+        <f>IF(beta_raw!A25="","",beta_raw!A25)</f>
         <v/>
       </c>
       <c r="B25" t="str">
@@ -6902,7 +6953,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>IF(beta!A26="","",beta!A26)</f>
+        <f>IF(beta_raw!A26="","",beta_raw!A26)</f>
         <v/>
       </c>
       <c r="B26" t="str">
@@ -6952,7 +7003,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>IF(beta!A27="","",beta!A27)</f>
+        <f>IF(beta_raw!A27="","",beta_raw!A27)</f>
         <v/>
       </c>
       <c r="B27" t="str">
@@ -7002,7 +7053,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f>IF(beta!A28="","",beta!A28)</f>
+        <f>IF(beta_raw!A28="","",beta_raw!A28)</f>
         <v/>
       </c>
       <c r="B28" t="str">
@@ -7052,7 +7103,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f>IF(beta!A29="","",beta!A29)</f>
+        <f>IF(beta_raw!A29="","",beta_raw!A29)</f>
         <v/>
       </c>
       <c r="B29" t="str">
@@ -7102,7 +7153,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>IF(beta!A30="","",beta!A30)</f>
+        <f>IF(beta_raw!A30="","",beta_raw!A30)</f>
         <v/>
       </c>
       <c r="B30" t="str">
@@ -7152,7 +7203,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f>IF(beta!A31="","",beta!A31)</f>
+        <f>IF(beta_raw!A31="","",beta_raw!A31)</f>
         <v/>
       </c>
       <c r="B31" t="str">
@@ -7202,73 +7253,73 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>IF(beta!A32="","",beta!A32)</f>
+        <f>IF(beta_raw!A32="","",beta_raw!A32)</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f>IF(beta!A33="","",beta!A33)</f>
+        <f>IF(beta_raw!A33="","",beta_raw!A33)</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f>IF(beta!A34="","",beta!A34)</f>
+        <f>IF(beta_raw!A34="","",beta_raw!A34)</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f>IF(beta!A35="","",beta!A35)</f>
+        <f>IF(beta_raw!A35="","",beta_raw!A35)</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f>IF(beta!A36="","",beta!A36)</f>
+        <f>IF(beta_raw!A36="","",beta_raw!A36)</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>IF(beta!A37="","",beta!A37)</f>
+        <f>IF(beta_raw!A37="","",beta_raw!A37)</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f>IF(beta!A38="","",beta!A38)</f>
+        <f>IF(beta_raw!A38="","",beta_raw!A38)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>IF(beta!A39="","",beta!A39)</f>
+        <f>IF(beta_raw!A39="","",beta_raw!A39)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f>IF(beta!A40="","",beta!A40)</f>
+        <f>IF(beta_raw!A40="","",beta_raw!A40)</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <f>IF(beta!A41="","",beta!A41)</f>
+        <f>IF(beta_raw!A41="","",beta_raw!A41)</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f>IF(beta!A42="","",beta!A42)</f>
+        <f>IF(beta_raw!A42="","",beta_raw!A42)</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f>IF(beta!A43="","",beta!A43)</f>
+        <f>IF(beta_raw!A43="","",beta_raw!A43)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
more progress towards running an experimental design
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-01.xlsx
+++ b/data/metapopulation-inputs-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2CC4FB-C343-D94B-B96D-1954599D8FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7C008A-98CB-1245-8FBB-F795DE9639DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="4" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="relative-mixing" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameters!$A$1:$G$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameters!$A$1:$F$24</definedName>
     <definedName name="c_">parameters!$B$6</definedName>
     <definedName name="C_surv">parameters!$B$12</definedName>
     <definedName name="days_to_adjust_NPI">parameters!$B$8</definedName>
@@ -60,11 +60,20 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={AA1D9824-023F-4443-9617-3E967B6A10FE}</author>
     <author>tc={E3294B68-B3C5-4A43-B614-3E4CB6542780}</author>
     <author>tc={3844B481-F1F1-B448-A37D-14DB0AD39FFD}</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{E3294B68-B3C5-4A43-B614-3E4CB6542780}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{AA1D9824-023F-4443-9617-3E967B6A10FE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These *are not* used in the code, they are here solely for our reference. The code itself specifies the values for these parameters.</t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="1" shapeId="0" xr:uid="{E3294B68-B3C5-4A43-B614-3E4CB6542780}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +83,7 @@
     This is the maximum prevalence the hospital system can possibly take.</t>
       </text>
     </comment>
-    <comment ref="B22" authorId="1" shapeId="0" xr:uid="{3844B481-F1F1-B448-A37D-14DB0AD39FFD}">
+    <comment ref="B22" authorId="2" shapeId="0" xr:uid="{3844B481-F1F1-B448-A37D-14DB0AD39FFD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>setting</t>
   </si>
@@ -196,9 +205,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>distribution</t>
-  </si>
-  <si>
     <t>jurisdiction</t>
   </si>
   <si>
@@ -404,6 +410,12 @@
   </si>
   <si>
     <t>transmissibility multiplicative factor used for scenario analysis. Multiplies over the beta matrix.</t>
+  </si>
+  <si>
+    <t>L_max</t>
+  </si>
+  <si>
+    <t>maximum intervention level.</t>
   </si>
 </sst>
 </file>
@@ -416,7 +428,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -437,6 +449,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -467,7 +493,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -481,6 +507,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -804,6 +831,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2023-09-13T14:17:26.59" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{AA1D9824-023F-4443-9617-3E967B6A10FE}">
+    <text>These *are not* used in the code, they are here solely for our reference. The code itself specifies the values for these parameters.</text>
+  </threadedComment>
   <threadedComment ref="B21" dT="2023-07-31T14:58:28.36" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{E3294B68-B3C5-4A43-B614-3E4CB6542780}">
     <text>60% baseline utilization * 2.38 hospital beds per 1000 people</text>
   </threadedComment>
@@ -876,10 +906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,54 +917,51 @@
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="92.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>17</v>
       </c>
       <c r="B2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <f>1/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -943,235 +970,235 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5">
         <v>0.01</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4">
         <f>35*10^5</f>
         <v>3500000</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>29</v>
       </c>
       <c r="B11" s="3">
         <v>5000</v>
       </c>
       <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>31</v>
       </c>
       <c r="B12" s="3">
         <v>10000000</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>2.5</v>
       </c>
       <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>36</v>
       </c>
       <c r="B14" s="7">
         <v>0.05</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="9">
         <v>0.02</v>
       </c>
       <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
         <v>44</v>
       </c>
-      <c r="G15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="11">
         <v>0.5</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="12">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="10">
         <f>0.7*2.38/1000/B15</f>
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="10">
         <f>B21*0.9</f>
         <v>7.4969999999999995E-2</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>1.5</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24">
         <v>279113</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25">
         <v>13.8</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -1182,13 +1209,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1200,44 +1227,55 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29">
         <v>1000</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>83</v>
       </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G24" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}"/>
+  <autoFilter ref="A1:F24" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -1262,24 +1300,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>6.0000000000000001E-3</v>
@@ -1296,7 +1334,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>0.13300000000000001</v>
@@ -1313,7 +1351,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>0.65500000000000003</v>
@@ -1330,7 +1368,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <f>0.219</f>
@@ -1382,10 +1420,10 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1438,7 +1476,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1555,7 +1593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D10A5E8-0BB5-4C43-827E-A5AF4D063B7C}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+    <sheetView zoomScale="169" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1563,7 +1601,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:T1">TRANSPOSE(A2:A20)</f>
@@ -7340,7 +7378,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:T1">TRANSPOSE(A2:A20)</f>

</xml_diff>